<commit_message>
Rename Variables in "Paying Taxes"
R was automatically renaming column headings in the "paying taxes" data because they were not unique for each column. However, the renaming was done in a different way on Daniel's vs. Elke's computer, so the code kept breaking. To fix the problem, the column headings were changed directly in the xlsx file.
</commit_message>
<xml_diff>
--- a/source_data/pwc_paying_taxes.xlsx
+++ b/source_data/pwc_paying_taxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ADAC36-FD44-4B4B-8645-B2E5613A599A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC975C3-6FF9-47B6-9B44-E80D31ECBE6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{67DB5D24-15D0-4B11-9A12-31369FF8C4D2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{67DB5D24-15D0-4B11-9A12-31369FF8C4D2}"/>
   </bookViews>
   <sheets>
     <sheet name="All 2018-2004 " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="280">
   <si>
     <t>Economy</t>
   </si>
@@ -672,6 +672,207 @@
   </si>
   <si>
     <t>Korea</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>corporate_time_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> labor_time_2018</t>
+  </si>
+  <si>
+    <t>consumption_time_2018</t>
+  </si>
+  <si>
+    <t>total_time_2018</t>
+  </si>
+  <si>
+    <t>profit_payments_2018</t>
+  </si>
+  <si>
+    <t>labor_payments_2018</t>
+  </si>
+  <si>
+    <t>other_payments_2018</t>
+  </si>
+  <si>
+    <t>total_payments_2018</t>
+  </si>
+  <si>
+    <t>corporate_time_2017</t>
+  </si>
+  <si>
+    <t>labor_time_2017</t>
+  </si>
+  <si>
+    <t>consumption_time_2017</t>
+  </si>
+  <si>
+    <t>total_time_2017</t>
+  </si>
+  <si>
+    <t>profit_payments_2017</t>
+  </si>
+  <si>
+    <t>labor_payments_2017</t>
+  </si>
+  <si>
+    <t>other_payments_2017</t>
+  </si>
+  <si>
+    <t>total_payments_2017</t>
+  </si>
+  <si>
+    <t>corporate_time_2016</t>
+  </si>
+  <si>
+    <t>labor_time_2016</t>
+  </si>
+  <si>
+    <t>consumption_time_2016</t>
+  </si>
+  <si>
+    <t>total_time_2016</t>
+  </si>
+  <si>
+    <t>profit_payments_2016</t>
+  </si>
+  <si>
+    <t>labor_payments_2016</t>
+  </si>
+  <si>
+    <t>other_payments_2016</t>
+  </si>
+  <si>
+    <t>total_payments_2016</t>
+  </si>
+  <si>
+    <t>corporate_time_2015</t>
+  </si>
+  <si>
+    <t>labor_time_2015</t>
+  </si>
+  <si>
+    <t>consumption_time_2015</t>
+  </si>
+  <si>
+    <t>total_time_2015</t>
+  </si>
+  <si>
+    <t>profit_payments_2015</t>
+  </si>
+  <si>
+    <t>labor_payments_2015</t>
+  </si>
+  <si>
+    <t>other_payments_2015</t>
+  </si>
+  <si>
+    <t>total_payments_2015</t>
+  </si>
+  <si>
+    <t>corporate_time_2014</t>
+  </si>
+  <si>
+    <t>labor_time_2014</t>
+  </si>
+  <si>
+    <t>consumption_time_2014</t>
+  </si>
+  <si>
+    <t>total_time_2014</t>
+  </si>
+  <si>
+    <t>profit_payments_2014</t>
+  </si>
+  <si>
+    <t>labor_payments_2014</t>
+  </si>
+  <si>
+    <t>other_payments_2014</t>
+  </si>
+  <si>
+    <t>total_payments_2014</t>
+  </si>
+  <si>
+    <t>corporate_time_2013</t>
+  </si>
+  <si>
+    <t>labor_time_2013</t>
+  </si>
+  <si>
+    <t>consumption_time_2013</t>
+  </si>
+  <si>
+    <t>total_time_2013</t>
+  </si>
+  <si>
+    <t>profit_payments_2013</t>
+  </si>
+  <si>
+    <t>labor_payments_2013</t>
+  </si>
+  <si>
+    <t>other_payments_2013</t>
+  </si>
+  <si>
+    <t>total_payments_2013</t>
+  </si>
+  <si>
+    <t>corporate_time_2012</t>
+  </si>
+  <si>
+    <t>labor_time_2012</t>
+  </si>
+  <si>
+    <t>consumption_time_2012</t>
+  </si>
+  <si>
+    <t>total_time_2012</t>
+  </si>
+  <si>
+    <t>profit_payments_2012</t>
+  </si>
+  <si>
+    <t>labor_payments_2012</t>
+  </si>
+  <si>
+    <t>other_payments_2012</t>
+  </si>
+  <si>
+    <t>total_payments_2012</t>
+  </si>
+  <si>
+    <t>corporate_time_2011</t>
+  </si>
+  <si>
+    <t>labor_time_2011</t>
+  </si>
+  <si>
+    <t>consumption_time_2011</t>
+  </si>
+  <si>
+    <t>total_time_2011</t>
+  </si>
+  <si>
+    <t>profit_payments_2011</t>
+  </si>
+  <si>
+    <t>labor_payments_2011</t>
+  </si>
+  <si>
+    <t>other_payments_2011</t>
+  </si>
+  <si>
+    <t>total_payments_2011</t>
   </si>
 </sst>
 </file>
@@ -1485,218 +1686,224 @@
   <dimension ref="B1:DT197"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
+      <selection pane="bottomRight" activeCell="BI1" sqref="BI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.73046875" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="124" width="9.28515625" customWidth="1"/>
+    <col min="5" max="8" width="9.265625" customWidth="1"/>
+    <col min="9" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="124" width="9.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:124" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="G1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="H1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="I1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="J1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="K1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="L1" s="3">
-        <v>2018</v>
-      </c>
-      <c r="M1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="N1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="O1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="P1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="R1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="S1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="T1" s="3">
-        <v>2017</v>
-      </c>
-      <c r="U1">
-        <v>2016</v>
-      </c>
-      <c r="V1">
-        <v>2016</v>
-      </c>
-      <c r="W1">
-        <v>2016</v>
-      </c>
-      <c r="X1">
-        <v>2016</v>
-      </c>
-      <c r="Y1">
-        <v>2016</v>
-      </c>
-      <c r="Z1">
-        <v>2016</v>
-      </c>
-      <c r="AA1">
-        <v>2016</v>
-      </c>
-      <c r="AB1">
-        <v>2016</v>
-      </c>
-      <c r="AC1">
-        <v>2015</v>
-      </c>
-      <c r="AD1">
-        <v>2015</v>
-      </c>
-      <c r="AE1">
-        <v>2015</v>
-      </c>
-      <c r="AF1">
-        <v>2015</v>
-      </c>
-      <c r="AG1">
-        <v>2015</v>
-      </c>
-      <c r="AH1">
-        <v>2015</v>
-      </c>
-      <c r="AI1">
-        <v>2015</v>
-      </c>
-      <c r="AJ1">
-        <v>2015</v>
-      </c>
-      <c r="AK1">
-        <v>2014</v>
-      </c>
-      <c r="AL1">
-        <v>2014</v>
-      </c>
-      <c r="AM1">
-        <v>2014</v>
-      </c>
-      <c r="AN1">
-        <v>2014</v>
-      </c>
-      <c r="AO1">
-        <v>2014</v>
-      </c>
-      <c r="AP1">
-        <v>2014</v>
-      </c>
-      <c r="AQ1">
-        <v>2014</v>
-      </c>
-      <c r="AR1">
-        <v>2014</v>
-      </c>
-      <c r="AS1">
-        <v>2013</v>
-      </c>
-      <c r="AT1">
-        <v>2013</v>
-      </c>
-      <c r="AU1">
-        <v>2013</v>
-      </c>
-      <c r="AV1">
-        <v>2013</v>
-      </c>
-      <c r="AW1">
-        <v>2013</v>
-      </c>
-      <c r="AX1">
-        <v>2013</v>
-      </c>
-      <c r="AY1">
-        <v>2013</v>
-      </c>
-      <c r="AZ1">
-        <v>2013</v>
-      </c>
-      <c r="BA1">
-        <v>2012</v>
-      </c>
-      <c r="BB1">
-        <v>2012</v>
-      </c>
-      <c r="BC1">
-        <v>2012</v>
-      </c>
-      <c r="BD1">
-        <v>2012</v>
-      </c>
-      <c r="BE1">
-        <v>2012</v>
-      </c>
-      <c r="BF1">
-        <v>2012</v>
-      </c>
-      <c r="BG1">
-        <v>2012</v>
-      </c>
-      <c r="BH1">
-        <v>2012</v>
-      </c>
-      <c r="BI1">
-        <v>2011</v>
-      </c>
-      <c r="BJ1">
-        <v>2011</v>
-      </c>
-      <c r="BK1">
-        <v>2011</v>
-      </c>
-      <c r="BL1">
-        <v>2011</v>
-      </c>
-      <c r="BM1">
-        <v>2011</v>
-      </c>
-      <c r="BN1">
-        <v>2011</v>
-      </c>
-      <c r="BO1">
-        <v>2011</v>
-      </c>
-      <c r="BP1">
-        <v>2011</v>
+    <row r="1" spans="2:124" x14ac:dyDescent="0.45">
+      <c r="B1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="U1" t="s">
+        <v>232</v>
+      </c>
+      <c r="V1" t="s">
+        <v>233</v>
+      </c>
+      <c r="W1" t="s">
+        <v>234</v>
+      </c>
+      <c r="X1" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>238</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>241</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>248</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>250</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>263</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>264</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>265</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>266</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>267</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>268</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>269</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>270</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>271</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>272</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>273</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>274</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>275</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>276</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>277</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>278</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>279</v>
       </c>
       <c r="BQ1">
         <v>2010</v>
@@ -1867,7 +2074,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="2" spans="2:124" ht="48" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:124" ht="46.5" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2238,7 +2445,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B3" s="39" t="s">
         <v>3</v>
       </c>
@@ -2609,7 +2816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B4" s="39" t="s">
         <v>6</v>
       </c>
@@ -2980,7 +3187,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B5" s="39" t="s">
         <v>9</v>
       </c>
@@ -3351,7 +3558,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B6" s="39" t="s">
         <v>11</v>
       </c>
@@ -3722,7 +3929,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B7" s="39" t="s">
         <v>13</v>
       </c>
@@ -4093,7 +4300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B8" s="39" t="s">
         <v>16</v>
       </c>
@@ -4464,7 +4671,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B9" s="39" t="s">
         <v>18</v>
       </c>
@@ -4835,7 +5042,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B10" s="39" t="s">
         <v>19</v>
       </c>
@@ -5206,7 +5413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B11" s="39" t="s">
         <v>20</v>
       </c>
@@ -5577,7 +5784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B12" s="39" t="s">
         <v>22</v>
       </c>
@@ -5948,7 +6155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B13" s="39" t="s">
         <v>23</v>
       </c>
@@ -6287,7 +6494,7 @@
       <c r="DS13" s="42"/>
       <c r="DT13" s="42"/>
     </row>
-    <row r="14" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B14" s="39" t="s">
         <v>24</v>
       </c>
@@ -6626,7 +6833,7 @@
       <c r="DS14" s="42"/>
       <c r="DT14" s="42"/>
     </row>
-    <row r="15" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B15" s="43" t="s">
         <v>26</v>
       </c>
@@ -6997,7 +7204,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B16" s="39" t="s">
         <v>27</v>
       </c>
@@ -7272,7 +7479,7 @@
       <c r="DS16" s="42"/>
       <c r="DT16" s="42"/>
     </row>
-    <row r="17" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B17" s="39" t="s">
         <v>28</v>
       </c>
@@ -7643,7 +7850,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B18" s="39" t="s">
         <v>29</v>
       </c>
@@ -8014,7 +8221,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B19" s="39" t="s">
         <v>30</v>
       </c>
@@ -8385,7 +8592,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B20" s="39" t="s">
         <v>31</v>
       </c>
@@ -8756,7 +8963,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B21" s="39" t="s">
         <v>32</v>
       </c>
@@ -9127,7 +9334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B22" s="39" t="s">
         <v>33</v>
       </c>
@@ -9498,7 +9705,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B23" s="39" t="s">
         <v>34</v>
       </c>
@@ -9869,7 +10076,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B24" s="39" t="s">
         <v>35</v>
       </c>
@@ -10240,7 +10447,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B25" s="43" t="s">
         <v>36</v>
       </c>
@@ -10611,7 +10818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B26" s="39" t="s">
         <v>37</v>
       </c>
@@ -10966,7 +11173,7 @@
       <c r="DS26" s="42"/>
       <c r="DT26" s="42"/>
     </row>
-    <row r="27" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B27" s="39" t="s">
         <v>38</v>
       </c>
@@ -11337,7 +11544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B28" s="39" t="s">
         <v>39</v>
       </c>
@@ -11708,7 +11915,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B29" s="39" t="s">
         <v>40</v>
       </c>
@@ -12079,7 +12286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B30" s="39" t="s">
         <v>41</v>
       </c>
@@ -12450,7 +12657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B31" s="39" t="s">
         <v>42</v>
       </c>
@@ -12821,7 +13028,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B32" s="39" t="s">
         <v>43</v>
       </c>
@@ -13192,7 +13399,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B33" s="39" t="s">
         <v>44</v>
       </c>
@@ -13563,7 +13770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B34" s="39" t="s">
         <v>46</v>
       </c>
@@ -13934,7 +14141,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B35" s="39" t="s">
         <v>47</v>
       </c>
@@ -14305,7 +14512,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B36" s="39" t="s">
         <v>48</v>
       </c>
@@ -14676,7 +14883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B37" s="43" t="s">
         <v>49</v>
       </c>
@@ -15047,7 +15254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B38" s="39" t="s">
         <v>50</v>
       </c>
@@ -15418,7 +15625,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B39" s="39" t="s">
         <v>51</v>
       </c>
@@ -15789,7 +15996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B40" s="39" t="s">
         <v>52</v>
       </c>
@@ -16160,7 +16367,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B41" s="39" t="s">
         <v>53</v>
       </c>
@@ -16531,7 +16738,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B42" s="39" t="s">
         <v>54</v>
       </c>
@@ -16902,7 +17109,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B43" s="39" t="s">
         <v>55</v>
       </c>
@@ -17273,7 +17480,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B44" s="39" t="s">
         <v>56</v>
       </c>
@@ -17644,7 +17851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="2:124" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:124" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="39" t="s">
         <v>57</v>
       </c>
@@ -17967,7 +18174,7 @@
       <c r="DS45" s="42"/>
       <c r="DT45" s="42"/>
     </row>
-    <row r="46" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B46" s="39" t="s">
         <v>58</v>
       </c>
@@ -18338,7 +18545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B47" s="39" t="s">
         <v>59</v>
       </c>
@@ -18709,7 +18916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B48" s="39" t="s">
         <v>60</v>
       </c>
@@ -19080,7 +19287,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B49" s="39" t="s">
         <v>61</v>
       </c>
@@ -19451,7 +19658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B50" s="39" t="s">
         <v>62</v>
       </c>
@@ -19822,7 +20029,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B51" s="39" t="s">
         <v>63</v>
       </c>
@@ -20193,7 +20400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B52" s="39" t="s">
         <v>64</v>
       </c>
@@ -20564,7 +20771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B53" s="39" t="s">
         <v>65</v>
       </c>
@@ -20935,7 +21142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B54" s="39" t="s">
         <v>66</v>
       </c>
@@ -21306,7 +21513,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B55" s="39" t="s">
         <v>67</v>
       </c>
@@ -21677,7 +21884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B56" s="39" t="s">
         <v>68</v>
       </c>
@@ -22048,7 +22255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B57" s="39" t="s">
         <v>69</v>
       </c>
@@ -22419,7 +22626,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B58" s="39" t="s">
         <v>70</v>
       </c>
@@ -22790,7 +22997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B59" s="39" t="s">
         <v>71</v>
       </c>
@@ -23161,7 +23368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B60" s="39" t="s">
         <v>72</v>
       </c>
@@ -23532,7 +23739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B61" s="39" t="s">
         <v>73</v>
       </c>
@@ -23903,7 +24110,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B62" s="39" t="s">
         <v>74</v>
       </c>
@@ -24274,7 +24481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B63" s="39" t="s">
         <v>75</v>
       </c>
@@ -24645,7 +24852,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B64" s="39" t="s">
         <v>76</v>
       </c>
@@ -25016,7 +25223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B65" s="39" t="s">
         <v>77</v>
       </c>
@@ -25387,7 +25594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B66" s="39" t="s">
         <v>78</v>
       </c>
@@ -25758,7 +25965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B67" s="39" t="s">
         <v>79</v>
       </c>
@@ -26129,7 +26336,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B68" s="39" t="s">
         <v>80</v>
       </c>
@@ -26500,7 +26707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B69" s="39" t="s">
         <v>81</v>
       </c>
@@ -26871,7 +27078,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B70" s="39" t="s">
         <v>82</v>
       </c>
@@ -27242,7 +27449,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B71" s="39" t="s">
         <v>83</v>
       </c>
@@ -27613,7 +27820,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B72" s="39" t="s">
         <v>84</v>
       </c>
@@ -27984,7 +28191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B73" s="39" t="s">
         <v>85</v>
       </c>
@@ -28355,7 +28562,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B74" s="39" t="s">
         <v>86</v>
       </c>
@@ -28726,7 +28933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="75" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B75" s="39" t="s">
         <v>87</v>
       </c>
@@ -29097,7 +29304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B76" s="39" t="s">
         <v>88</v>
       </c>
@@ -29468,7 +29675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B77" s="39" t="s">
         <v>89</v>
       </c>
@@ -29839,7 +30046,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B78" s="43" t="s">
         <v>90</v>
       </c>
@@ -30210,7 +30417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B79" s="43" t="s">
         <v>91</v>
       </c>
@@ -30581,7 +30788,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B80" s="39" t="s">
         <v>92</v>
       </c>
@@ -30952,7 +31159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B81" s="39" t="s">
         <v>93</v>
       </c>
@@ -31323,7 +31530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B82" s="39" t="s">
         <v>94</v>
       </c>
@@ -31694,7 +31901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B83" s="39" t="s">
         <v>95</v>
       </c>
@@ -32065,7 +32272,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B84" s="39" t="s">
         <v>96</v>
       </c>
@@ -32436,7 +32643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B85" s="39" t="s">
         <v>97</v>
       </c>
@@ -32807,7 +33014,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B86" s="43" t="s">
         <v>98</v>
       </c>
@@ -33178,7 +33385,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B87" s="39" t="s">
         <v>99</v>
       </c>
@@ -33549,7 +33756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B88" s="39" t="s">
         <v>100</v>
       </c>
@@ -33920,7 +34127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B89" s="39" t="s">
         <v>101</v>
       </c>
@@ -34291,7 +34498,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="90" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B90" s="39" t="s">
         <v>102</v>
       </c>
@@ -34662,7 +34869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B91" s="39" t="s">
         <v>212</v>
       </c>
@@ -35033,7 +35240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B92" s="39" t="s">
         <v>103</v>
       </c>
@@ -35356,7 +35563,7 @@
       <c r="DS92" s="42"/>
       <c r="DT92" s="42"/>
     </row>
-    <row r="93" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B93" s="39" t="s">
         <v>104</v>
       </c>
@@ -35727,7 +35934,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B94" s="39" t="s">
         <v>105</v>
       </c>
@@ -36098,7 +36305,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B95" s="39" t="s">
         <v>106</v>
       </c>
@@ -36469,7 +36676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B96" s="39" t="s">
         <v>107</v>
       </c>
@@ -36840,7 +37047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B97" s="39" t="s">
         <v>108</v>
       </c>
@@ -37211,7 +37418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B98" s="39" t="s">
         <v>109</v>
       </c>
@@ -37582,7 +37789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B99" s="39" t="s">
         <v>110</v>
       </c>
@@ -37937,7 +38144,7 @@
       <c r="DS99" s="42"/>
       <c r="DT99" s="42"/>
     </row>
-    <row r="100" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B100" s="39" t="s">
         <v>111</v>
       </c>
@@ -38196,7 +38403,7 @@
       <c r="DS100" s="42"/>
       <c r="DT100" s="42"/>
     </row>
-    <row r="101" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B101" s="39" t="s">
         <v>112</v>
       </c>
@@ -38567,7 +38774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B102" s="39" t="s">
         <v>113</v>
       </c>
@@ -38922,7 +39129,7 @@
       <c r="DS102" s="42"/>
       <c r="DT102" s="42"/>
     </row>
-    <row r="103" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B103" s="39" t="s">
         <v>114</v>
       </c>
@@ -39293,7 +39500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B104" s="39" t="s">
         <v>115</v>
       </c>
@@ -39664,7 +39871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B105" s="39" t="s">
         <v>116</v>
       </c>
@@ -40035,7 +40242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B106" s="39" t="s">
         <v>117</v>
       </c>
@@ -40406,7 +40613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B107" s="39" t="s">
         <v>118</v>
       </c>
@@ -40777,7 +40984,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B108" s="39" t="s">
         <v>119</v>
       </c>
@@ -41052,7 +41259,7 @@
       <c r="DS108" s="42"/>
       <c r="DT108" s="42"/>
     </row>
-    <row r="109" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B109" s="39" t="s">
         <v>120</v>
       </c>
@@ -41423,7 +41630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B110" s="39" t="s">
         <v>121</v>
       </c>
@@ -41794,7 +42001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B111" s="39" t="s">
         <v>122</v>
       </c>
@@ -42165,7 +42372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B112" s="43" t="s">
         <v>123</v>
       </c>
@@ -42536,7 +42743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B113" s="39" t="s">
         <v>124</v>
       </c>
@@ -42907,7 +43114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B114" s="39" t="s">
         <v>125</v>
       </c>
@@ -43278,7 +43485,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="115" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B115" s="39" t="s">
         <v>126</v>
       </c>
@@ -43649,7 +43856,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B116" s="39" t="s">
         <v>127</v>
       </c>
@@ -44004,7 +44211,7 @@
       <c r="DS116" s="42"/>
       <c r="DT116" s="42"/>
     </row>
-    <row r="117" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B117" s="39" t="s">
         <v>128</v>
       </c>
@@ -44375,7 +44582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B118" s="39" t="s">
         <v>129</v>
       </c>
@@ -44746,7 +44953,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B119" s="39" t="s">
         <v>130</v>
       </c>
@@ -45005,7 +45212,7 @@
       <c r="DS119" s="42"/>
       <c r="DT119" s="42"/>
     </row>
-    <row r="120" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B120" s="39" t="s">
         <v>131</v>
       </c>
@@ -45376,7 +45583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B121" s="39" t="s">
         <v>132</v>
       </c>
@@ -45747,7 +45954,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B122" s="39" t="s">
         <v>133</v>
       </c>
@@ -46118,7 +46325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B123" s="39" t="s">
         <v>134</v>
       </c>
@@ -46489,7 +46696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B124" s="39" t="s">
         <v>135</v>
       </c>
@@ -46860,7 +47067,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="125" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B125" s="39" t="s">
         <v>136</v>
       </c>
@@ -47231,7 +47438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="126" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B126" s="43" t="s">
         <v>137</v>
       </c>
@@ -47602,7 +47809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B127" s="39" t="s">
         <v>138</v>
       </c>
@@ -47973,7 +48180,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B128" s="39" t="s">
         <v>139</v>
       </c>
@@ -48344,7 +48551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B129" s="39" t="s">
         <v>140</v>
       </c>
@@ -48715,7 +48922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B130" s="43" t="s">
         <v>141</v>
       </c>
@@ -49086,7 +49293,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="131" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B131" s="39" t="s">
         <v>142</v>
       </c>
@@ -49457,7 +49664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B132" s="39" t="s">
         <v>143</v>
       </c>
@@ -49828,7 +50035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="133" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B133" s="39" t="s">
         <v>144</v>
       </c>
@@ -50199,7 +50406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B134" s="39" t="s">
         <v>145</v>
       </c>
@@ -50570,7 +50777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="135" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B135" s="39" t="s">
         <v>146</v>
       </c>
@@ -50941,7 +51148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B136" s="39" t="s">
         <v>147</v>
       </c>
@@ -51312,7 +51519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="137" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B137" s="39" t="s">
         <v>148</v>
       </c>
@@ -51683,7 +51890,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="138" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B138" s="39" t="s">
         <v>149</v>
       </c>
@@ -52054,7 +52261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B139" s="39" t="s">
         <v>150</v>
       </c>
@@ -52425,7 +52632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B140" s="39" t="s">
         <v>151</v>
       </c>
@@ -52764,7 +52971,7 @@
       <c r="DS140" s="42"/>
       <c r="DT140" s="42"/>
     </row>
-    <row r="141" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B141" s="39" t="s">
         <v>152</v>
       </c>
@@ -53135,7 +53342,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="142" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B142" s="43" t="s">
         <v>153</v>
       </c>
@@ -53506,7 +53713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B143" s="39" t="s">
         <v>154</v>
       </c>
@@ -53877,7 +54084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="144" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B144" s="39" t="s">
         <v>155</v>
       </c>
@@ -54248,7 +54455,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B145" s="39" t="s">
         <v>156</v>
       </c>
@@ -54507,7 +54714,7 @@
       <c r="DS145" s="42"/>
       <c r="DT145" s="42"/>
     </row>
-    <row r="146" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B146" s="39" t="s">
         <v>157</v>
       </c>
@@ -54878,7 +55085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B147" s="39" t="s">
         <v>158</v>
       </c>
@@ -55249,7 +55456,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B148" s="39" t="s">
         <v>159</v>
       </c>
@@ -55620,7 +55827,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B149" s="39" t="s">
         <v>160</v>
       </c>
@@ -55991,7 +56198,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="150" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B150" s="39" t="s">
         <v>161</v>
       </c>
@@ -56362,7 +56569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="151" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B151" s="39" t="s">
         <v>162</v>
       </c>
@@ -56733,7 +56940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B152" s="39" t="s">
         <v>163</v>
       </c>
@@ -57104,7 +57311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B153" s="39" t="s">
         <v>164</v>
       </c>
@@ -57475,7 +57682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B154" s="39" t="s">
         <v>165</v>
       </c>
@@ -57846,7 +58053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B155" s="39" t="s">
         <v>166</v>
       </c>
@@ -58217,7 +58424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="156" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B156" s="39" t="s">
         <v>167</v>
       </c>
@@ -58588,7 +58795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="157" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B157" s="39" t="s">
         <v>168</v>
       </c>
@@ -58847,7 +59054,7 @@
       <c r="DS157" s="42"/>
       <c r="DT157" s="42"/>
     </row>
-    <row r="158" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B158" s="39" t="s">
         <v>169</v>
       </c>
@@ -59218,7 +59425,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B159" s="39" t="s">
         <v>170</v>
       </c>
@@ -59589,7 +59796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="160" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B160" s="39" t="s">
         <v>171</v>
       </c>
@@ -59960,7 +60167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="161" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B161" s="39" t="s">
         <v>172</v>
       </c>
@@ -60331,7 +60538,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="162" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B162" s="39" t="s">
         <v>173</v>
       </c>
@@ -60702,7 +60909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B163" s="39" t="s">
         <v>174</v>
       </c>
@@ -61073,7 +61280,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="164" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B164" s="39" t="s">
         <v>175</v>
       </c>
@@ -61444,7 +61651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B165" s="39" t="s">
         <v>176</v>
       </c>
@@ -61815,7 +62022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B166" s="39" t="s">
         <v>177</v>
       </c>
@@ -62186,7 +62393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B167" s="39" t="s">
         <v>178</v>
       </c>
@@ -62557,7 +62764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B168" s="39" t="s">
         <v>179</v>
       </c>
@@ -62928,7 +63135,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B169" s="39" t="s">
         <v>180</v>
       </c>
@@ -63299,7 +63506,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B170" s="39" t="s">
         <v>181</v>
       </c>
@@ -63670,7 +63877,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="171" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B171" s="39" t="s">
         <v>182</v>
       </c>
@@ -64041,7 +64248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B172" s="39" t="s">
         <v>183</v>
       </c>
@@ -64412,7 +64619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B173" s="39" t="s">
         <v>184</v>
       </c>
@@ -64783,7 +64990,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="174" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B174" s="39" t="s">
         <v>185</v>
       </c>
@@ -65154,7 +65361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B175" s="39" t="s">
         <v>186</v>
       </c>
@@ -65525,7 +65732,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="176" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B176" s="39" t="s">
         <v>187</v>
       </c>
@@ -65896,7 +66103,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B177" s="39" t="s">
         <v>188</v>
       </c>
@@ -66267,7 +66474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B178" s="39" t="s">
         <v>189</v>
       </c>
@@ -66638,7 +66845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="179" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B179" s="39" t="s">
         <v>190</v>
       </c>
@@ -67009,7 +67216,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="180" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B180" s="39" t="s">
         <v>191</v>
       </c>
@@ -67380,7 +67587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B181" s="39" t="s">
         <v>192</v>
       </c>
@@ -67751,7 +67958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B182" s="43" t="s">
         <v>193</v>
       </c>
@@ -68122,7 +68329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B183" s="39" t="s">
         <v>194</v>
       </c>
@@ -68493,7 +68700,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="184" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B184" s="39" t="s">
         <v>195</v>
       </c>
@@ -68864,7 +69071,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="185" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B185" s="39" t="s">
         <v>196</v>
       </c>
@@ -69235,7 +69442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B186" s="39" t="s">
         <v>197</v>
       </c>
@@ -69606,7 +69813,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="187" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B187" s="39" t="s">
         <v>198</v>
       </c>
@@ -69977,7 +70184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="188" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B188" s="39" t="s">
         <v>199</v>
       </c>
@@ -70348,7 +70555,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="189" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B189" s="39" t="s">
         <v>200</v>
       </c>
@@ -70719,7 +70926,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="190" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B190" s="39" t="s">
         <v>201</v>
       </c>
@@ -71090,7 +71297,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="191" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B191" s="39" t="s">
         <v>202</v>
       </c>
@@ -71461,7 +71668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="192" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:124" x14ac:dyDescent="0.45">
       <c r="E192" s="44"/>
       <c r="F192" s="44"/>
       <c r="G192" s="44"/>
@@ -71583,7 +71790,7 @@
       <c r="DS192" s="42"/>
       <c r="DT192" s="42"/>
     </row>
-    <row r="193" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:124" x14ac:dyDescent="0.45">
       <c r="E193" s="44"/>
       <c r="F193" s="44"/>
       <c r="G193" s="44"/>
@@ -71705,7 +71912,7 @@
       <c r="DS193" s="42"/>
       <c r="DT193" s="42"/>
     </row>
-    <row r="194" spans="2:124" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:124" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B194" s="46" t="s">
         <v>203</v>
       </c>
@@ -72072,7 +72279,7 @@
         <v>34.522988505747129</v>
       </c>
     </row>
-    <row r="195" spans="2:124" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:124" s="71" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B195"/>
       <c r="C195"/>
       <c r="D195"/>
@@ -72197,7 +72404,7 @@
       <c r="DS195" s="42"/>
       <c r="DT195" s="42"/>
     </row>
-    <row r="196" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:124" x14ac:dyDescent="0.45">
       <c r="E196" s="44"/>
       <c r="F196" s="44"/>
       <c r="G196" s="44"/>
@@ -72319,7 +72526,7 @@
       <c r="DS196" s="44"/>
       <c r="DT196" s="44"/>
     </row>
-    <row r="197" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:124" x14ac:dyDescent="0.45">
       <c r="B197" s="75"/>
       <c r="E197" s="44"/>
       <c r="F197" s="44"/>

</xml_diff>